<commit_message>
Last change working. Wihtout Interrupt
</commit_message>
<xml_diff>
--- a/docs/Motorrad CANbus.xlsx
+++ b/docs/Motorrad CANbus.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Arduino\BMW Canbus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\repos\github\mentxo\arduino-f800gs-canbus\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3F8B71-4DE3-4E11-B717-DF98071E0369}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68043FBB-9412-4A0C-83A8-1A91C6CAD052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4347,6 +4347,9 @@
     <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4368,9 +4371,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6677,13 +6677,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="85" t="s">
         <v>326</v>
       </c>
       <c r="B13" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="84" t="s">
+      <c r="C13" s="85" t="s">
         <v>327</v>
       </c>
       <c r="D13" s="26" t="s">
@@ -6691,11 +6691,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="83"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="83"/>
+      <c r="C14" s="84"/>
       <c r="D14" s="26" t="s">
         <v>284</v>
       </c>
@@ -6808,7 +6808,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="85" t="s">
         <v>335</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -6822,7 +6822,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="24" t="s">
         <v>37</v>
       </c>
@@ -6834,7 +6834,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83"/>
+      <c r="A4" s="84"/>
       <c r="B4" s="24"/>
       <c r="C4" s="43" t="s">
         <v>338</v>
@@ -6844,7 +6844,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="84" t="s">
+      <c r="A5" s="85" t="s">
         <v>339</v>
       </c>
       <c r="B5" s="24" t="s">
@@ -6858,7 +6858,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="24"/>
       <c r="C6" s="43" t="s">
         <v>341</v>
@@ -6868,7 +6868,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="84" t="s">
+      <c r="A7" s="85" t="s">
         <v>342</v>
       </c>
       <c r="B7" s="24" t="s">
@@ -6882,7 +6882,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="83"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="24" t="s">
         <v>40</v>
       </c>
@@ -6894,7 +6894,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="83"/>
+      <c r="A9" s="84"/>
       <c r="B9" s="24"/>
       <c r="C9" s="43" t="s">
         <v>345</v>
@@ -7652,33 +7652,33 @@
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="10"/>
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
+      <c r="E2" s="79"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="80"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10"/>
       <c r="B3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="78"/>
-      <c r="E3" s="78"/>
-      <c r="F3" s="78"/>
-      <c r="G3" s="78"/>
-      <c r="H3" s="78"/>
-      <c r="I3" s="78"/>
-      <c r="J3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="80"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="10"/>
@@ -7720,16 +7720,16 @@
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
-      <c r="C9" s="80" t="s">
+      <c r="C9" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="81"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="82"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
@@ -7762,18 +7762,18 @@
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="78"/>
-      <c r="E11" s="78"/>
-      <c r="F11" s="81"/>
-      <c r="G11" s="80" t="s">
+      <c r="D11" s="79"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="H11" s="78"/>
-      <c r="I11" s="78"/>
-      <c r="J11" s="81"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="79"/>
+      <c r="J11" s="82"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
@@ -8509,20 +8509,20 @@
       <c r="D10" s="53" t="s">
         <v>436</v>
       </c>
-      <c r="E10" s="85" t="s">
+      <c r="E10" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="83"/>
-      <c r="G10" s="86" t="s">
+      <c r="F10" s="84"/>
+      <c r="G10" s="87" t="s">
         <v>437</v>
       </c>
-      <c r="H10" s="83"/>
-      <c r="I10" s="83"/>
-      <c r="J10" s="83"/>
-      <c r="K10" s="83"/>
-      <c r="L10" s="83"/>
-      <c r="M10" s="83"/>
-      <c r="N10" s="83"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="84"/>
+      <c r="J10" s="84"/>
+      <c r="K10" s="84"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
+      <c r="N10" s="84"/>
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
@@ -8749,7 +8749,7 @@
       <c r="A16" s="1"/>
       <c r="B16" s="38"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="86" t="s">
+      <c r="D16" s="87" t="s">
         <v>443</v>
       </c>
       <c r="E16" s="54" t="s">
@@ -8797,7 +8797,7 @@
       <c r="A17" s="1"/>
       <c r="B17" s="38"/>
       <c r="C17" s="1"/>
-      <c r="D17" s="83"/>
+      <c r="D17" s="84"/>
       <c r="E17" s="54" t="s">
         <v>445</v>
       </c>
@@ -10738,8 +10738,8 @@
   </sheetPr>
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -11032,16 +11032,16 @@
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="44">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C24">
         <f>(HEX2DEC(B25)*256 + HEX2DEC(B24))/4</f>
-        <v>0</v>
+        <v>1369.25</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -28815,7 +28815,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="83" t="s">
         <v>245</v>
       </c>
       <c r="B4" s="34" t="s">
@@ -28829,7 +28829,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="83"/>
+      <c r="A5" s="84"/>
       <c r="B5" s="34" t="s">
         <v>39</v>
       </c>
@@ -28841,7 +28841,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83"/>
+      <c r="A6" s="84"/>
       <c r="B6" s="34"/>
       <c r="C6" s="35" t="s">
         <v>248</v>
@@ -29316,7 +29316,7 @@
       <c r="B8" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="87" t="s">
+      <c r="C8" s="77" t="s">
         <v>283</v>
       </c>
       <c r="D8" s="26" t="s">

</xml_diff>